<commit_message>
spring 2018 spreadsheet all set. also added wint, cd, and qfr requirements.
</commit_message>
<xml_diff>
--- a/class_schedules_spring_2018/AFRICANA STUDIES (AAST).xlsx
+++ b/class_schedules_spring_2018/AFRICANA STUDIES (AAST).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="153">
   <si>
     <t>072</t>
   </si>
@@ -64,18 +64,48 @@
     <t>502F</t>
   </si>
   <si>
+    <t>502</t>
+  </si>
+  <si>
     <t>502H</t>
   </si>
   <si>
     <t>995F</t>
   </si>
   <si>
+    <t>995</t>
+  </si>
+  <si>
     <t>995H</t>
   </si>
   <si>
     <t>01</t>
   </si>
   <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
     <t>18093</t>
   </si>
   <si>
@@ -124,15 +154,96 @@
     <t>16977</t>
   </si>
   <si>
+    <t>16978</t>
+  </si>
+  <si>
+    <t>16979</t>
+  </si>
+  <si>
+    <t>16980</t>
+  </si>
+  <si>
+    <t>16981</t>
+  </si>
+  <si>
+    <t>16982</t>
+  </si>
+  <si>
+    <t>16983</t>
+  </si>
+  <si>
+    <t>17916</t>
+  </si>
+  <si>
     <t>16970</t>
   </si>
   <si>
+    <t>16971</t>
+  </si>
+  <si>
+    <t>16972</t>
+  </si>
+  <si>
+    <t>16973</t>
+  </si>
+  <si>
+    <t>16974</t>
+  </si>
+  <si>
+    <t>16975</t>
+  </si>
+  <si>
+    <t>17917</t>
+  </si>
+  <si>
     <t>16546</t>
   </si>
   <si>
+    <t>16547</t>
+  </si>
+  <si>
+    <t>16548</t>
+  </si>
+  <si>
+    <t>16549</t>
+  </si>
+  <si>
+    <t>16550</t>
+  </si>
+  <si>
+    <t>16551</t>
+  </si>
+  <si>
+    <t>17918</t>
+  </si>
+  <si>
+    <t>18982</t>
+  </si>
+  <si>
     <t>16539</t>
   </si>
   <si>
+    <t>16540</t>
+  </si>
+  <si>
+    <t>16541</t>
+  </si>
+  <si>
+    <t>16542</t>
+  </si>
+  <si>
+    <t>16543</t>
+  </si>
+  <si>
+    <t>16544</t>
+  </si>
+  <si>
+    <t>17919</t>
+  </si>
+  <si>
+    <t>18983</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
@@ -142,82 +253,109 @@
     <t>F</t>
   </si>
   <si>
-    <t>Blues Aesthetic: Cont/Transfrm R</t>
-  </si>
-  <si>
-    <t>Intro to Africana Studies TR</t>
-  </si>
-  <si>
-    <t>History of the Caribbean: II TR</t>
-  </si>
-  <si>
-    <t>Intr African-American Music II T</t>
-  </si>
-  <si>
-    <t>West African Dance II TR</t>
-  </si>
-  <si>
-    <t>South Africa Since 1948 TR</t>
-  </si>
-  <si>
-    <t>Choreography:Culture Tradition TR</t>
-  </si>
-  <si>
-    <t>Radical Thinkers and Movements TR</t>
-  </si>
-  <si>
-    <t>Africana Popular Culture TR</t>
-  </si>
-  <si>
-    <t>Black English and Voice MW</t>
+    <t>R</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>MWF</t>
+  </si>
+  <si>
+    <t>Blues Aesthetic: Cont/Transfrm</t>
+  </si>
+  <si>
+    <t>Intro to Africana Studies</t>
+  </si>
+  <si>
+    <t>History of the Caribbean: II</t>
+  </si>
+  <si>
+    <t>Intr African American Music II</t>
+  </si>
+  <si>
+    <t>West African Dance II</t>
+  </si>
+  <si>
+    <t>South Africa Since 1948</t>
+  </si>
+  <si>
+    <t>Choreography:Culture Tradition</t>
+  </si>
+  <si>
+    <t>Radical Thinkers and Movements</t>
+  </si>
+  <si>
+    <t>Africana Popular Culture</t>
+  </si>
+  <si>
+    <t>Black English and Voice</t>
   </si>
   <si>
     <t>Black Arts Workshop TR</t>
   </si>
   <si>
-    <t>Intermediate Seminar W</t>
-  </si>
-  <si>
-    <t>Caribbean Empire &amp; Resistance M</t>
-  </si>
-  <si>
-    <t>Djapo Dance @ Oberlin TR</t>
-  </si>
-  <si>
-    <t>Soc of African-Amer Community MWF</t>
-  </si>
-  <si>
-    <t>Senior Honors -</t>
-  </si>
-  <si>
-    <t>Private Reading -</t>
-  </si>
-  <si>
-    <t>0100-0250pm</t>
-  </si>
-  <si>
-    <t>0300-0420pm</t>
-  </si>
-  <si>
-    <t>1100-1220pm</t>
-  </si>
-  <si>
-    <t>0700-0900pm</t>
-  </si>
-  <si>
-    <t>0835-0950am</t>
-  </si>
-  <si>
-    <t>0930-1050am</t>
-  </si>
-  <si>
-    <t>0230-0420pm</t>
-  </si>
-  <si>
-    <t>1000-1150am</t>
-  </si>
-  <si>
-    <t>1000-1050am</t>
+    <t>Intermediate Seminar</t>
+  </si>
+  <si>
+    <t>Caribbean Empire &amp; Resistance</t>
+  </si>
+  <si>
+    <t>Djapo Dance @ Oberlin</t>
+  </si>
+  <si>
+    <t>Soc of African Amer Community</t>
+  </si>
+  <si>
+    <t>Senior Honors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Honors </t>
+  </si>
+  <si>
+    <t>Private Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private Reading </t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>0300</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>0700</t>
+  </si>
+  <si>
+    <t>0835</t>
+  </si>
+  <si>
+    <t>0930</t>
+  </si>
+  <si>
+    <t>0230</t>
+  </si>
+  <si>
+    <t>1150am</t>
   </si>
   <si>
     <t>Full</t>
@@ -226,6 +364,30 @@
     <t>Half</t>
   </si>
   <si>
+    <t>0250pm</t>
+  </si>
+  <si>
+    <t>0420pm</t>
+  </si>
+  <si>
+    <t>1220pm</t>
+  </si>
+  <si>
+    <t>0900pm</t>
+  </si>
+  <si>
+    <t>0950am</t>
+  </si>
+  <si>
+    <t>1050am</t>
+  </si>
+  <si>
+    <t>WARN</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
     <t>ART2</t>
   </si>
   <si>
@@ -235,13 +397,10 @@
     <t>CBIB</t>
   </si>
   <si>
-    <t>WARN</t>
-  </si>
-  <si>
     <t>KING</t>
   </si>
   <si>
-    <t>TBA</t>
+    <t>ST3</t>
   </si>
   <si>
     <t>050</t>
@@ -262,7 +421,7 @@
     <t>239</t>
   </si>
   <si>
-    <t>ST3</t>
+    <t>Jackson</t>
   </si>
   <si>
     <t>337</t>
@@ -292,13 +451,28 @@
     <t>Johns Gillian</t>
   </si>
   <si>
-    <t>Jackson-Smith Caro</t>
+    <t>Smith Caro</t>
   </si>
   <si>
     <t>Gadsby Meredith</t>
   </si>
   <si>
     <t>White Clovis</t>
+  </si>
+  <si>
+    <t>Emeka Justin</t>
+  </si>
+  <si>
+    <t>Opoku Darko</t>
+  </si>
+  <si>
+    <t>Sharpley Miriam</t>
+  </si>
+  <si>
+    <t>Raynor Candice</t>
+  </si>
+  <si>
+    <t>Staff A&amp;S</t>
   </si>
 </sst>
 </file>
@@ -656,13 +830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -693,8 +867,14 @@
       <c r="K1" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -702,34 +882,40 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="J2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="M2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -737,34 +923,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>125</v>
+      </c>
+      <c r="L3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -772,34 +964,40 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="K4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>125</v>
+      </c>
+      <c r="L4" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -807,34 +1005,40 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="K5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>126</v>
+      </c>
+      <c r="L5" t="s">
+        <v>130</v>
+      </c>
+      <c r="M5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -842,34 +1046,40 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>122</v>
+      </c>
+      <c r="L6" t="s">
+        <v>131</v>
+      </c>
+      <c r="M6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -877,34 +1087,40 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="K7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>127</v>
+      </c>
+      <c r="L7" t="s">
+        <v>132</v>
+      </c>
+      <c r="M7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -912,34 +1128,40 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="J8" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>122</v>
+      </c>
+      <c r="L8" t="s">
+        <v>133</v>
+      </c>
+      <c r="M8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -947,34 +1169,40 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="J9" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="K9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>125</v>
+      </c>
+      <c r="L9" t="s">
+        <v>129</v>
+      </c>
+      <c r="M9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -982,34 +1210,40 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="I10" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>127</v>
+      </c>
+      <c r="L10" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1017,34 +1251,40 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="J11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" t="s">
         <v>2</v>
       </c>
-      <c r="K11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="M11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1052,34 +1292,40 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="J12" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="K12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>128</v>
+      </c>
+      <c r="L12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1087,34 +1333,40 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="J13" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="K13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>127</v>
+      </c>
+      <c r="L13" t="s">
+        <v>136</v>
+      </c>
+      <c r="M13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1122,34 +1374,40 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="J14" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="K14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>125</v>
+      </c>
+      <c r="L14" t="s">
+        <v>129</v>
+      </c>
+      <c r="M14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1157,34 +1415,40 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="J15" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="K15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>122</v>
+      </c>
+      <c r="L15" t="s">
+        <v>133</v>
+      </c>
+      <c r="M15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1192,34 +1456,40 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="K16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>127</v>
+      </c>
+      <c r="L16" t="s">
+        <v>137</v>
+      </c>
+      <c r="M16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1227,34 +1497,34 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="J17" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="K17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>123</v>
+      </c>
+      <c r="L17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1262,101 +1532,1058 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="J18" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>123</v>
+      </c>
+      <c r="L18" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
-      </c>
-      <c r="I19" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="K19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>123</v>
+      </c>
+      <c r="L19" t="s">
+        <v>123</v>
+      </c>
+      <c r="M19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" t="s">
+        <v>114</v>
+      </c>
+      <c r="K20" t="s">
+        <v>123</v>
+      </c>
+      <c r="L20" t="s">
+        <v>123</v>
+      </c>
+      <c r="M20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" t="s">
+        <v>123</v>
+      </c>
+      <c r="L21" t="s">
+        <v>135</v>
+      </c>
+      <c r="M21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" t="s">
+        <v>114</v>
+      </c>
+      <c r="K22" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22" t="s">
+        <v>123</v>
+      </c>
+      <c r="M22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" t="s">
+        <v>102</v>
+      </c>
+      <c r="J23" t="s">
+        <v>114</v>
+      </c>
+      <c r="K23" t="s">
+        <v>123</v>
+      </c>
+      <c r="L23" t="s">
+        <v>123</v>
+      </c>
+      <c r="M23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" t="s">
+        <v>114</v>
+      </c>
+      <c r="K24" t="s">
+        <v>123</v>
+      </c>
+      <c r="L24" t="s">
+        <v>123</v>
+      </c>
+      <c r="M24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" t="s">
+        <v>115</v>
+      </c>
+      <c r="K25" t="s">
+        <v>123</v>
+      </c>
+      <c r="L25" t="s">
+        <v>123</v>
+      </c>
+      <c r="M25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" t="s">
+        <v>115</v>
+      </c>
+      <c r="K26" t="s">
+        <v>123</v>
+      </c>
+      <c r="L26" t="s">
+        <v>123</v>
+      </c>
+      <c r="M26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" t="s">
+        <v>115</v>
+      </c>
+      <c r="K27" t="s">
+        <v>123</v>
+      </c>
+      <c r="L27" t="s">
+        <v>123</v>
+      </c>
+      <c r="M27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" t="s">
+        <v>115</v>
+      </c>
+      <c r="K28" t="s">
+        <v>123</v>
+      </c>
+      <c r="L28" t="s">
+        <v>123</v>
+      </c>
+      <c r="M28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" t="s">
+        <v>103</v>
+      </c>
+      <c r="I29" t="s">
+        <v>115</v>
+      </c>
+      <c r="J29" t="s">
+        <v>123</v>
+      </c>
+      <c r="K29" t="s">
+        <v>123</v>
+      </c>
+      <c r="L29" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30" t="s">
+        <v>115</v>
+      </c>
+      <c r="K30" t="s">
+        <v>123</v>
+      </c>
+      <c r="L30" t="s">
+        <v>123</v>
+      </c>
+      <c r="M30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" t="s">
+        <v>115</v>
+      </c>
+      <c r="K31" t="s">
+        <v>123</v>
+      </c>
+      <c r="L31" t="s">
+        <v>123</v>
+      </c>
+      <c r="M31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" t="s">
+        <v>104</v>
+      </c>
+      <c r="J32" t="s">
+        <v>114</v>
+      </c>
+      <c r="K32" t="s">
+        <v>123</v>
+      </c>
+      <c r="L32" t="s">
+        <v>123</v>
+      </c>
+      <c r="M32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" t="s">
+        <v>104</v>
+      </c>
+      <c r="J33" t="s">
+        <v>114</v>
+      </c>
+      <c r="K33" t="s">
+        <v>123</v>
+      </c>
+      <c r="L33" t="s">
+        <v>123</v>
+      </c>
+      <c r="M33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" t="s">
+        <v>114</v>
+      </c>
+      <c r="K34" t="s">
+        <v>123</v>
+      </c>
+      <c r="L34" t="s">
+        <v>123</v>
+      </c>
+      <c r="M34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35" t="s">
+        <v>114</v>
+      </c>
+      <c r="K35" t="s">
+        <v>123</v>
+      </c>
+      <c r="L35" t="s">
+        <v>123</v>
+      </c>
+      <c r="M35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36" t="s">
+        <v>114</v>
+      </c>
+      <c r="J36" t="s">
+        <v>123</v>
+      </c>
+      <c r="K36" t="s">
+        <v>123</v>
+      </c>
+      <c r="L36" t="s">
+        <v>135</v>
+      </c>
+      <c r="M36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" t="s">
+        <v>104</v>
+      </c>
+      <c r="J37" t="s">
+        <v>114</v>
+      </c>
+      <c r="K37" t="s">
+        <v>123</v>
+      </c>
+      <c r="L37" t="s">
+        <v>123</v>
+      </c>
+      <c r="M37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H38" t="s">
+        <v>104</v>
+      </c>
+      <c r="J38" t="s">
+        <v>114</v>
+      </c>
+      <c r="K38" t="s">
+        <v>123</v>
+      </c>
+      <c r="L38" t="s">
+        <v>123</v>
+      </c>
+      <c r="M38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" t="s">
+        <v>104</v>
+      </c>
+      <c r="J39" t="s">
+        <v>114</v>
+      </c>
+      <c r="K39" t="s">
+        <v>123</v>
+      </c>
+      <c r="L39" t="s">
+        <v>123</v>
+      </c>
+      <c r="M39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="E20" t="s">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" t="s">
+        <v>78</v>
+      </c>
+      <c r="H40" t="s">
+        <v>104</v>
+      </c>
+      <c r="J40" t="s">
+        <v>115</v>
+      </c>
+      <c r="K40" t="s">
+        <v>123</v>
+      </c>
+      <c r="L40" t="s">
+        <v>123</v>
+      </c>
+      <c r="M40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" t="s">
+        <v>78</v>
+      </c>
+      <c r="H41" t="s">
+        <v>104</v>
+      </c>
+      <c r="J41" t="s">
+        <v>115</v>
+      </c>
+      <c r="K41" t="s">
+        <v>123</v>
+      </c>
+      <c r="L41" t="s">
+        <v>123</v>
+      </c>
+      <c r="M41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="F20" t="s">
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" t="s">
+        <v>104</v>
+      </c>
+      <c r="J42" t="s">
+        <v>115</v>
+      </c>
+      <c r="K42" t="s">
+        <v>123</v>
+      </c>
+      <c r="L42" t="s">
+        <v>123</v>
+      </c>
+      <c r="M42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="G20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" t="s">
+        <v>104</v>
+      </c>
+      <c r="J43" t="s">
+        <v>115</v>
+      </c>
+      <c r="K43" t="s">
+        <v>123</v>
+      </c>
+      <c r="L43" t="s">
+        <v>123</v>
+      </c>
+      <c r="M43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" t="s">
+        <v>104</v>
+      </c>
+      <c r="J44" t="s">
+        <v>115</v>
+      </c>
+      <c r="K44" t="s">
+        <v>123</v>
+      </c>
+      <c r="L44" t="s">
+        <v>123</v>
+      </c>
+      <c r="M44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" t="s">
+        <v>78</v>
+      </c>
+      <c r="H45" t="s">
+        <v>104</v>
+      </c>
+      <c r="J45" t="s">
+        <v>115</v>
+      </c>
+      <c r="K45" t="s">
+        <v>123</v>
+      </c>
+      <c r="L45" t="s">
+        <v>123</v>
+      </c>
+      <c r="M45" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" t="s">
+        <v>115</v>
+      </c>
+      <c r="J46" t="s">
+        <v>123</v>
+      </c>
+      <c r="K46" t="s">
+        <v>123</v>
+      </c>
+      <c r="L46" t="s">
+        <v>135</v>
+      </c>
+      <c r="M46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" t="s">
         <v>75</v>
       </c>
-      <c r="J20" t="s">
-        <v>75</v>
-      </c>
-      <c r="K20" t="s">
-        <v>90</v>
+      <c r="E47" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" t="s">
+        <v>104</v>
+      </c>
+      <c r="J47" t="s">
+        <v>115</v>
+      </c>
+      <c r="K47" t="s">
+        <v>123</v>
+      </c>
+      <c r="L47" t="s">
+        <v>123</v>
+      </c>
+      <c r="M47" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>